<commit_message>
feat: implemented excel import experimentally
</commit_message>
<xml_diff>
--- a/model/heath_construction_data_template.xlsx
+++ b/model/heath_construction_data_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PhD\02_Development\heath\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chalmers-my.sharepoint.com/personal/sawen_chalmers_se/Documents/Documents/PhD/development/heath/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86C74456-B45D-4F70-907A-84EAAA0349CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{86C74456-B45D-4F70-907A-84EAAA0349CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB2502BF-3B37-47A9-875A-09A93AB9D975}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{70233ACE-60CF-4097-9719-0F8765C618DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{70233ACE-60CF-4097-9719-0F8765C618DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>display_name</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>gwp_a5_1</t>
+  </si>
+  <si>
+    <t>Mineral wool</t>
+  </si>
+  <si>
+    <t>Insulation</t>
+  </si>
+  <si>
+    <t>Construction 1</t>
+  </si>
+  <si>
+    <t>Construction 2</t>
   </si>
 </sst>
 </file>
@@ -167,6 +179,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -486,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640CFC9D-E50B-4074-9655-1931FC733B64}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,6 +543,41 @@
       </c>
       <c r="K1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>0.7</v>
+      </c>
+      <c r="C2">
+        <v>1030</v>
+      </c>
+      <c r="D2">
+        <v>0.7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>0.9</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.35</v>
+      </c>
+      <c r="J2">
+        <v>0.05</v>
+      </c>
+      <c r="K2">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>
@@ -536,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BE8CF0-66BE-43F4-BC51-AC2C71A94C89}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,6 +636,34 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>0.3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>